<commit_message>
Update Matriz de Involucrado de Espirulina- ultimo.xlsx
</commit_message>
<xml_diff>
--- a/Otros Trabajos Encargados/Matriz de Involucrado de Espirulina- ultimo.xlsx
+++ b/Otros Trabajos Encargados/Matriz de Involucrado de Espirulina- ultimo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ULT. TRABAJOS ENCARGADOS - ESPIRULINA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioORFEI\Proyecto-034-ESPIRULINA\Otros Trabajos Encargados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="MAT. DE INVOLUCRADOS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'MAT. DE INVOLUCRADOS'!$A$1:$H$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'MAT. DE INVOLUCRADOS'!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>GRUPOS  INVOLUCRADOS</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>prover la Instalacion  del  módulo de producción de Espirulina para promover la innovación tecnológica.</t>
+  </si>
+  <si>
+    <t>DIRECCION  REGIONAL DE EDUCACION  DE APURIMAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efectos de la desnutricion  en el aprendizaje  escolar  en la provincia de Abancay - Region de Apurimac </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asumir  la formalizacion  juridica   de convenio    para la afectacion de uso de terreno  de una  1 Ha.  para la Instalacion fisica  del proyecto.  </t>
   </si>
 </sst>
 </file>
@@ -257,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -380,19 +395,62 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,32 +459,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -437,26 +477,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -739,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J22"/>
+  <dimension ref="B3:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,60 +781,60 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="2:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="28"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="29"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="2:10" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
@@ -831,231 +855,246 @@
       <c r="G9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="33"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="37" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="33"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="2:10" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="33"/>
-    </row>
-    <row r="12" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C13" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D13" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F13" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G13" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="2:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="4" t="s">
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="2:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="24"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="33"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="15"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F15" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="2:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="2:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F16" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="39"/>
-    </row>
-    <row r="16" spans="2:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="39"/>
-    </row>
-    <row r="17" spans="2:8" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="28"/>
+    </row>
+    <row r="17" spans="2:8" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+    <row r="18" spans="2:8" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="39"/>
-    </row>
-    <row r="18" spans="2:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
+      <c r="H18" s="28"/>
+    </row>
+    <row r="19" spans="2:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C19" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G19" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="39"/>
-    </row>
-    <row r="19" spans="2:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="39"/>
-    </row>
-    <row r="20" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
+      <c r="H19" s="28"/>
+    </row>
+    <row r="20" spans="2:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="23"/>
       <c r="C20" s="26"/>
       <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="28"/>
+    </row>
+    <row r="21" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="24"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="33"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
     <mergeCell ref="B3:H4"/>
-    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -1065,6 +1104,12 @@
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:G8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="H16:H20"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="39" orientation="portrait" r:id="rId1"/>

</xml_diff>